<commit_message>
Righting up progress review
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S23130205\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC42F17-9391-4DB7-8B21-383B7FFCD25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26368A4F-9278-45CF-8D7A-987822C0FCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD616266-8E6B-4F13-ADD5-149E74AA759E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Poster and Viva</t>
+  </si>
+  <si>
+    <t>Time Added</t>
+  </si>
+  <si>
+    <t>Time Taken</t>
   </si>
 </sst>
 </file>
@@ -99,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +115,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -138,7 +156,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFE712E-3B8E-4151-83FB-333889E333A9}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +650,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -642,9 +662,7 @@
       <c r="C4" s="3">
         <v>45999</v>
       </c>
-      <c r="G4" s="6"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -656,11 +674,12 @@
       <c r="C5" s="3">
         <v>46055</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="7"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -672,8 +691,7 @@
       <c r="C6" s="3">
         <v>46076</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
     </row>
@@ -687,10 +705,6 @@
       <c r="C7" s="3">
         <v>46083</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
@@ -706,7 +720,6 @@
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="6"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -718,10 +731,8 @@
       <c r="C9" s="3">
         <v>46084</v>
       </c>
-      <c r="V9" s="6"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
-      <c r="Y9" s="6"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -734,9 +745,6 @@
         <v>46118</v>
       </c>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -765,6 +773,18 @@
       </c>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D15" s="6"/>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>